<commit_message>
Finished 2 problems from Lesson 3.1
</commit_message>
<xml_diff>
--- a/cheatsheets.xlsx
+++ b/cheatsheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEAD0EC-A6AF-4EB7-876C-0819258B900E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB97E03-14FF-4EDF-8383-F4A00E2C98A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="129">
   <si>
     <t>String.prototype.concat()</t>
   </si>
@@ -978,6 +978,9 @@
   </si>
   <si>
     <t>Array.prototype.some()</t>
+  </si>
+  <si>
+    <t>Array.prototype.endsWith()</t>
   </si>
 </sst>
 </file>
@@ -1582,8 +1585,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6970381E-85E7-4EC3-A462-564D376755FE}" name="Table3" displayName="Table3" ref="A1:F12" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A1:F12" xr:uid="{6970381E-85E7-4EC3-A462-564D376755FE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6970381E-85E7-4EC3-A462-564D376755FE}" name="Table3" displayName="Table3" ref="A1:F13" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A1:F13" xr:uid="{6970381E-85E7-4EC3-A462-564D376755FE}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{21BDCA9F-C8E8-44E9-9113-6FF65DE75A27}" name="Method or Property" dataDxfId="33" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{DA2C9FF2-B521-41D5-9DC9-20BDBA5FD225}" name="Required Parameters" dataDxfId="32"/>
@@ -1925,10 +1928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317FE35D-C95D-407B-8F83-74B4C8605AFC}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2159,6 +2162,16 @@
       <c r="E12" s="10"/>
       <c r="F12" s="1"/>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{5325B499-44BC-4090-A7DE-C6D54BB9B8FC}"/>
@@ -2172,11 +2185,12 @@
     <hyperlink ref="A10" r:id="rId9" xr:uid="{05008E9D-030F-4B61-B5D5-053BDFC3DABF}"/>
     <hyperlink ref="A11" r:id="rId10" xr:uid="{210EFA93-C283-42A9-B5F4-834FF7F5ECB1}"/>
     <hyperlink ref="A12" r:id="rId11" xr:uid="{305DD501-0060-4163-881D-F538A815689F}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{A4FA154E-3E60-4C81-BCAB-FA72E4E69FD4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Finish 5 problems from Lesson 3.3
</commit_message>
<xml_diff>
--- a/cheatsheets.xlsx
+++ b/cheatsheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB97E03-14FF-4EDF-8383-F4A00E2C98A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B90560-7505-4440-BD38-DA77F508F07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="131">
   <si>
     <t>String.prototype.concat()</t>
   </si>
@@ -980,7 +980,13 @@
     <t>Array.prototype.some()</t>
   </si>
   <si>
-    <t>Array.prototype.endsWith()</t>
+    <t>Array.prototype.every()</t>
+  </si>
+  <si>
+    <t>Array.prototype.flat()</t>
+  </si>
+  <si>
+    <t>String.prototype.endsWith()</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1051,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1068,6 +1074,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1076,91 +1083,6 @@
   <dxfs count="36">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1317,6 +1239,91 @@
         <scheme val="none"/>
       </font>
       <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1585,8 +1592,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6970381E-85E7-4EC3-A462-564D376755FE}" name="Table3" displayName="Table3" ref="A1:F13" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A1:F13" xr:uid="{6970381E-85E7-4EC3-A462-564D376755FE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6970381E-85E7-4EC3-A462-564D376755FE}" name="Table3" displayName="Table3" ref="A1:F14" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A1:F14" xr:uid="{6970381E-85E7-4EC3-A462-564D376755FE}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{21BDCA9F-C8E8-44E9-9113-6FF65DE75A27}" name="Method or Property" dataDxfId="33" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{DA2C9FF2-B521-41D5-9DC9-20BDBA5FD225}" name="Required Parameters" dataDxfId="32"/>
@@ -1630,36 +1637,36 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C6386E1-B398-466B-82BA-E318577D8786}" name="Table1" displayName="Table1" ref="A1:F12" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:F12" xr:uid="{2C6386E1-B398-466B-82BA-E318577D8786}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C6386E1-B398-466B-82BA-E318577D8786}" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F13" xr:uid="{2C6386E1-B398-466B-82BA-E318577D8786}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E12">
     <sortCondition ref="A1:A12"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7AAB2C99-B880-474D-8BD4-ACCC61A0DD35}" name="Method or Property" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{003EA47F-4174-4173-A8E7-07B0983D6587}" name="Required Parameters" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{25B19BFB-6938-4AC1-BD40-AC62A95EEF30}" name="Optional Parameters" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{B587D95F-A1EE-488A-953B-51382025636B}" name="Return Value" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{9483E40F-FB5C-490C-BCBA-5B1A036DED9F}" name="Notes" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{9551E13B-B219-45E3-A96D-A282A653EA1A}" name="Mutates?" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{7AAB2C99-B880-474D-8BD4-ACCC61A0DD35}" name="Method or Property" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{003EA47F-4174-4173-A8E7-07B0983D6587}" name="Required Parameters" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{25B19BFB-6938-4AC1-BD40-AC62A95EEF30}" name="Optional Parameters" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{B587D95F-A1EE-488A-953B-51382025636B}" name="Return Value" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{9483E40F-FB5C-490C-BCBA-5B1A036DED9F}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{9551E13B-B219-45E3-A96D-A282A653EA1A}" name="Mutates?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{47A7FEDA-DC9E-43D6-98F2-42E99BC9948E}" name="Table356" displayName="Table356" ref="A1:F6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{47A7FEDA-DC9E-43D6-98F2-42E99BC9948E}" name="Table356" displayName="Table356" ref="A1:F6" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:F6" xr:uid="{47A7FEDA-DC9E-43D6-98F2-42E99BC9948E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F6">
     <sortCondition ref="A1:A6"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{5B0B5271-1788-4B99-AFCD-7F5294032119}" name="Method or Property" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{9C61A5ED-BCE3-40CC-9188-ECDDB4F1003D}" name="Required Parameters" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{9CA527D0-2377-41A0-AF7F-8B6CA543BE4C}" name="Optional Parameters" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A381BA80-BA26-41D9-8A74-5AD78C9EF260}" name="Return Value" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{A0D7E78D-5CD4-4D82-9EFF-93401C37C7EC}" name="Notes" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{B7EFFAF9-97E3-456A-8A8E-184E291B3AE0}" name="Mutates?" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{9C61A5ED-BCE3-40CC-9188-ECDDB4F1003D}" name="Required Parameters" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{9CA527D0-2377-41A0-AF7F-8B6CA543BE4C}" name="Optional Parameters" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{A381BA80-BA26-41D9-8A74-5AD78C9EF260}" name="Return Value" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{A0D7E78D-5CD4-4D82-9EFF-93401C37C7EC}" name="Notes" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{B7EFFAF9-97E3-456A-8A8E-184E291B3AE0}" name="Mutates?" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1928,21 +1935,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317FE35D-C95D-407B-8F83-74B4C8605AFC}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>70</v>
       </c>
@@ -1962,7 +1969,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -1982,7 +1989,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>92</v>
       </c>
@@ -2002,7 +2009,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>97</v>
       </c>
@@ -2022,7 +2029,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>99</v>
       </c>
@@ -2042,7 +2049,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>104</v>
       </c>
@@ -2062,7 +2069,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>108</v>
       </c>
@@ -2082,7 +2089,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>113</v>
       </c>
@@ -2102,7 +2109,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>117</v>
       </c>
@@ -2122,7 +2129,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>121</v>
       </c>
@@ -2142,7 +2149,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>124</v>
       </c>
@@ -2152,7 +2159,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>127</v>
       </c>
@@ -2162,7 +2169,7 @@
       <c r="E12" s="10"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>128</v>
       </c>
@@ -2171,6 +2178,16 @@
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2185,12 +2202,13 @@
     <hyperlink ref="A10" r:id="rId9" xr:uid="{05008E9D-030F-4B61-B5D5-053BDFC3DABF}"/>
     <hyperlink ref="A11" r:id="rId10" xr:uid="{210EFA93-C283-42A9-B5F4-834FF7F5ECB1}"/>
     <hyperlink ref="A12" r:id="rId11" xr:uid="{305DD501-0060-4163-881D-F538A815689F}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{A4FA154E-3E60-4C81-BCAB-FA72E4E69FD4}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{0F2F6355-566D-42DD-8B85-57FD2E678959}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{32ED205C-E50A-4B81-AAC6-94F0344A67F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
   <tableParts count="1">
-    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2206,16 +2224,16 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>70</v>
       </c>
@@ -2235,7 +2253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>73</v>
       </c>
@@ -2255,7 +2273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>77</v>
       </c>
@@ -2275,7 +2293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>80</v>
       </c>
@@ -2295,7 +2313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>84</v>
       </c>
@@ -2315,7 +2333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>88</v>
       </c>
@@ -2359,14 +2377,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -2384,19 +2402,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>27</v>
       </c>
@@ -2420,14 +2438,14 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>49</v>
       </c>
@@ -2438,7 +2456,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>60</v>
       </c>
@@ -2447,7 +2465,7 @@
       </c>
       <c r="C2" s="10"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>62</v>
       </c>
@@ -2456,7 +2474,7 @@
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>54</v>
       </c>
@@ -2465,7 +2483,7 @@
       </c>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>53</v>
       </c>
@@ -2474,7 +2492,7 @@
       </c>
       <c r="C5" s="10"/>
     </row>
-    <row r="6" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>64</v>
       </c>
@@ -2485,7 +2503,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>66</v>
       </c>
@@ -2496,7 +2514,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>58</v>
       </c>
@@ -2505,7 +2523,7 @@
       </c>
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>56</v>
       </c>
@@ -2540,16 +2558,16 @@
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>70</v>
       </c>
@@ -2569,7 +2587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>72</v>
       </c>
@@ -2596,7 +2614,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2610,7 +2628,7 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2624,9 +2642,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>126</v>
       </c>
@@ -2638,29 +2656,29 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.26953125" customWidth="1"/>
-    <col min="3" max="3" width="25.54296875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="25.1796875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.54296875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.453125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="35.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>70</v>
       </c>
@@ -2681,7 +2699,7 @@
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -2702,7 +2720,7 @@
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -2723,7 +2741,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
@@ -2744,7 +2762,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>25</v>
       </c>
@@ -2765,7 +2783,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>33</v>
       </c>
@@ -2786,7 +2804,7 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
@@ -2807,7 +2825,7 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>38</v>
       </c>
@@ -2828,7 +2846,7 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
@@ -2849,7 +2867,7 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>43</v>
       </c>
@@ -2870,7 +2888,7 @@
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>45</v>
       </c>
@@ -2891,7 +2909,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>47</v>
       </c>
@@ -2911,6 +2929,16 @@
         <v>2</v>
       </c>
       <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2925,11 +2953,12 @@
     <hyperlink ref="A10" r:id="rId9" xr:uid="{9145286E-605A-46F1-9FC8-7C55A2D9E8D1}"/>
     <hyperlink ref="A11" r:id="rId10" xr:uid="{7ABA0E8D-8130-41AF-B8B4-5D0A0C5952FA}"/>
     <hyperlink ref="A12" r:id="rId11" xr:uid="{BA8CAEB8-7734-47C9-9CC1-760259A4B746}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{58C760F2-0E3E-4776-BACA-C3A8DE05352E}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId12"/>
+  <pageSetup orientation="landscape" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finish Find the Duplicate
</commit_message>
<xml_diff>
--- a/cheatsheets.xlsx
+++ b/cheatsheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B90560-7505-4440-BD38-DA77F508F07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5F5364-317F-4392-B6B5-27E08049D943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="131">
   <si>
     <t>String.prototype.concat()</t>
   </si>
@@ -1083,6 +1083,91 @@
   <dxfs count="36">
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1239,91 +1324,6 @@
         <scheme val="none"/>
       </font>
       <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1592,8 +1592,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6970381E-85E7-4EC3-A462-564D376755FE}" name="Table3" displayName="Table3" ref="A1:F14" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A1:F14" xr:uid="{6970381E-85E7-4EC3-A462-564D376755FE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6970381E-85E7-4EC3-A462-564D376755FE}" name="Table3" displayName="Table3" ref="A1:F16" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A1:F16" xr:uid="{6970381E-85E7-4EC3-A462-564D376755FE}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{21BDCA9F-C8E8-44E9-9113-6FF65DE75A27}" name="Method or Property" dataDxfId="33" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{DA2C9FF2-B521-41D5-9DC9-20BDBA5FD225}" name="Required Parameters" dataDxfId="32"/>
@@ -1637,36 +1637,36 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C6386E1-B398-466B-82BA-E318577D8786}" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C6386E1-B398-466B-82BA-E318577D8786}" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:F13" xr:uid="{2C6386E1-B398-466B-82BA-E318577D8786}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E12">
     <sortCondition ref="A1:A12"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7AAB2C99-B880-474D-8BD4-ACCC61A0DD35}" name="Method or Property" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{003EA47F-4174-4173-A8E7-07B0983D6587}" name="Required Parameters" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{25B19BFB-6938-4AC1-BD40-AC62A95EEF30}" name="Optional Parameters" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{B587D95F-A1EE-488A-953B-51382025636B}" name="Return Value" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{9483E40F-FB5C-490C-BCBA-5B1A036DED9F}" name="Notes" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{9551E13B-B219-45E3-A96D-A282A653EA1A}" name="Mutates?" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{7AAB2C99-B880-474D-8BD4-ACCC61A0DD35}" name="Method or Property" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{003EA47F-4174-4173-A8E7-07B0983D6587}" name="Required Parameters" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{25B19BFB-6938-4AC1-BD40-AC62A95EEF30}" name="Optional Parameters" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{B587D95F-A1EE-488A-953B-51382025636B}" name="Return Value" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{9483E40F-FB5C-490C-BCBA-5B1A036DED9F}" name="Notes" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{9551E13B-B219-45E3-A96D-A282A653EA1A}" name="Mutates?" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{47A7FEDA-DC9E-43D6-98F2-42E99BC9948E}" name="Table356" displayName="Table356" ref="A1:F6" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{47A7FEDA-DC9E-43D6-98F2-42E99BC9948E}" name="Table356" displayName="Table356" ref="A1:F6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:F6" xr:uid="{47A7FEDA-DC9E-43D6-98F2-42E99BC9948E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F6">
     <sortCondition ref="A1:A6"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{5B0B5271-1788-4B99-AFCD-7F5294032119}" name="Method or Property" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{9C61A5ED-BCE3-40CC-9188-ECDDB4F1003D}" name="Required Parameters" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{9CA527D0-2377-41A0-AF7F-8B6CA543BE4C}" name="Optional Parameters" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{A381BA80-BA26-41D9-8A74-5AD78C9EF260}" name="Return Value" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{A0D7E78D-5CD4-4D82-9EFF-93401C37C7EC}" name="Notes" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{B7EFFAF9-97E3-456A-8A8E-184E291B3AE0}" name="Mutates?" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{9C61A5ED-BCE3-40CC-9188-ECDDB4F1003D}" name="Required Parameters" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{9CA527D0-2377-41A0-AF7F-8B6CA543BE4C}" name="Optional Parameters" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A381BA80-BA26-41D9-8A74-5AD78C9EF260}" name="Return Value" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{A0D7E78D-5CD4-4D82-9EFF-93401C37C7EC}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{B7EFFAF9-97E3-456A-8A8E-184E291B3AE0}" name="Mutates?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1935,10 +1935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317FE35D-C95D-407B-8F83-74B4C8605AFC}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2188,6 +2188,26 @@
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2204,11 +2224,13 @@
     <hyperlink ref="A12" r:id="rId11" xr:uid="{305DD501-0060-4163-881D-F538A815689F}"/>
     <hyperlink ref="A13" r:id="rId12" xr:uid="{0F2F6355-566D-42DD-8B85-57FD2E678959}"/>
     <hyperlink ref="A14" r:id="rId13" xr:uid="{32ED205C-E50A-4B81-AAC6-94F0344A67F0}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{C2256E11-4F8F-4C3C-B463-2D859C92FB82}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{227B6C74-C703-464C-B30F-9E82FD06C08F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2658,11 +2680,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>